<commit_message>
updated the ai information json, added priority to the ai response selection
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,26 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rana\Documents\My stuff\coding\talkitover\Google Universal Sentence Encoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E76E0B-A613-47DE-9C12-56684B4B75C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA43961-5062-488B-8EFD-CDA1CA5DDBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="18315" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="1725" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exemplars" sheetId="1" r:id="rId1"/>
     <sheet name="thresholds" sheetId="2" r:id="rId2"/>
     <sheet name="responseAlreadyUsed" sheetId="3" r:id="rId3"/>
+    <sheet name="priority" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="295">
   <si>
     <t>Abuse</t>
   </si>
@@ -803,7 +813,115 @@
     <t>helpResponseAlreadyUsed</t>
   </si>
   <si>
-    <t>What sort of help would you like? (By the way I'm a pretty simple bot and I'm here to listen)</t>
+    <t>abuseResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>Addictions can be really tough. Could you say more about what it means for you?</t>
+  </si>
+  <si>
+    <t>["Just a quick reminder -- if there's any kind of abuse situation going on, or if you or anyone else is unsafe, please remember that I can't get help for you, so you would need to get help for yourself if you need it.", "And I'm programmed to err on the side of caution (i.e. I might accidentally give this response when it's not a clearly abusive situation, sorry about that). I didn't mean to interrupt the flow of this conversation, so please feel free to keep talking."]</t>
+  </si>
+  <si>
+    <t>If there's anything more about stress/anxiety/fear you want to explore, feel free to say more about that here</t>
+  </si>
+  <si>
+    <t>thisBotIsBadResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>I'm a simple bot, trying my best to listen and help. I won't always get it right (sorry about that) but I'm still here to listen</t>
+  </si>
+  <si>
+    <t>I don't know much about coronavirus or pandemics, but I can be here for you while you talk about it if that might help</t>
+  </si>
+  <si>
+    <t>iHaveDepressionResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>I think it's sad whenever anyone feels depression or anything like that</t>
+  </si>
+  <si>
+    <t>feelEmptyResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>I just wanted to pick up on the idea of emptiness. Feel free to say anything more about that?</t>
+  </si>
+  <si>
+    <t>Do keep telling me more. I'm definitely no expert on family or relationships or anything like that, but I hope talking about it is helping.</t>
+  </si>
+  <si>
+    <t>I'm sensing some negativity towards yourself, and that's really sad</t>
+  </si>
+  <si>
+    <t>If you're needing help, I can try to be useful by being a place for you to talk through what's on your mind</t>
+  </si>
+  <si>
+    <t>Hmm, sounds tough. Would you like to explore your options with me? I'll be here to listen</t>
+  </si>
+  <si>
+    <t>Sometimes issues like image and appearance can make us feel bad or cause self-esteem issues. That's really sad.</t>
+  </si>
+  <si>
+    <t>It's sad whenever anyone is lonely or is missing the connections to other people that are so important</t>
+  </si>
+  <si>
+    <t>I'm getting the sense of a lost, almost forlorn feeling from what you're saying</t>
+  </si>
+  <si>
+    <t>I'm sensing a certain level of feeling a bit overwhelmed, perhaps?</t>
+  </si>
+  <si>
+    <t>I'm sorry that things have got so had that you feel that way</t>
+  </si>
+  <si>
+    <t>Whenever someone has suicidal thoughts, that's always sad.</t>
+  </si>
+  <si>
+    <t>I'm sorry to hear about any sadness or upset that you might be having at the moment</t>
+  </si>
+  <si>
+    <t>I hope you don't me mentioning that everyone has value, everyone has worth.</t>
+  </si>
+  <si>
+    <t>familyProblemsResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>iHateMyselfResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>iDontKnowWhatToDoResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>imAnxiousResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>imAddictedResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>iHateCoronavirusResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>iHateHowILookResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>feelingLonelyResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>feelLostResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>feelOverwhelmedResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>makesMeWantToSelfHarmResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>imUpsetResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>imFeelingSuicidalResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>imUselessResponseAlreadyUsed</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1242,7 @@
   <dimension ref="A1:S82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,8 +2323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608A1981-5BEF-491A-9A06-8E0829FC9A3D}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,10 +2337,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,10 +2348,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,10 +2359,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,10 +2370,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2263,10 +2381,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="C5" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,10 +2392,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2285,10 +2403,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,10 +2414,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="C8" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,10 +2425,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>282</v>
       </c>
       <c r="C9" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2321,7 +2439,7 @@
         <v>257</v>
       </c>
       <c r="C10" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,10 +2447,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
       <c r="C11" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,10 +2458,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>287</v>
       </c>
       <c r="C12" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,10 +2469,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>257</v>
+        <v>288</v>
       </c>
       <c r="C13" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,10 +2480,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>257</v>
+        <v>289</v>
       </c>
       <c r="C14" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2373,10 +2491,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>290</v>
       </c>
       <c r="C15" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2384,10 +2502,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>257</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2395,10 +2513,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>257</v>
+        <v>293</v>
       </c>
       <c r="C17" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2406,10 +2524,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>257</v>
+        <v>292</v>
       </c>
       <c r="C18" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2417,10 +2535,180 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>257</v>
+        <v>294</v>
       </c>
       <c r="C19" t="s">
-        <v>258</v>
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022D9653-5E4C-42CB-9FC5-B0AC6900CD6F}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refined the ai a bit, added certain information to the stored data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rana\Documents\My stuff\coding\talkitover\Google Universal Sentence Encoder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rana\Documents\My stuff\coding\talkitover\talkitover2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA43961-5062-488B-8EFD-CDA1CA5DDBDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0514DAA0-ADBB-46A5-95EF-D68060009365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="1725" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4785" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exemplars" sheetId="1" r:id="rId1"/>
@@ -870,9 +870,6 @@
     <t>I'm sensing a certain level of feeling a bit overwhelmed, perhaps?</t>
   </si>
   <si>
-    <t>I'm sorry that things have got so had that you feel that way</t>
-  </si>
-  <si>
     <t>Whenever someone has suicidal thoughts, that's always sad.</t>
   </si>
   <si>
@@ -922,6 +919,9 @@
   </si>
   <si>
     <t>imUselessResponseAlreadyUsed</t>
+  </si>
+  <si>
+    <t>I'm sorry that things have got so hard that you feel that way</t>
   </si>
 </sst>
 </file>
@@ -2323,8 +2323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608A1981-5BEF-491A-9A06-8E0829FC9A3D}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,7 +2348,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C2" t="s">
         <v>259</v>
@@ -2359,7 +2359,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C3" t="s">
         <v>261</v>
@@ -2381,7 +2381,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" t="s">
         <v>264</v>
@@ -2414,7 +2414,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C8" t="s">
         <v>269</v>
@@ -2425,7 +2425,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C9" t="s">
         <v>270</v>
@@ -2447,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C11" t="s">
         <v>272</v>
@@ -2458,7 +2458,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C12" t="s">
         <v>273</v>
@@ -2469,7 +2469,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C13" t="s">
         <v>274</v>
@@ -2480,7 +2480,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C14" t="s">
         <v>275</v>
@@ -2491,7 +2491,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C15" t="s">
         <v>276</v>
@@ -2502,10 +2502,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C16" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,10 +2513,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2524,10 +2524,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2535,10 +2535,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>